<commit_message>
Frontend - Actualización de plantilla xlsx.
</commit_message>
<xml_diff>
--- a/WebAPI/wwwroot/Plantillas/EmergenciasPreviamenteCargadas.xlsx
+++ b/WebAPI/wwwroot/Plantillas/EmergenciasPreviamenteCargadas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CONAGUA\GitLab\sica\WebAPI\wwwroot\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1144C21-6E29-42C5-83E8-825FFB8EE221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFF4429-00C9-4AD0-9844-296101B0C7CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BDACBC7F-1DE3-4174-9935-405E203EC69D}"/>
   </bookViews>
@@ -27,14 +27,14 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Emergencias previamente cargadas</t>
+    <t>EMERGENCIAS PREVIAMENTE CARGADAS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,7 +44,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -59,8 +67,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -79,10 +86,10 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="40% - Énfasis4" xfId="1" builtinId="43"/>
+    <cellStyle name="Incorrecto" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -401,7 +408,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>

</xml_diff>